<commit_message>
Growth of functions done; working on recursive relations and height of recursive tree
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECBF37A-70AC-4ADA-B390-C9AAB858C269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B39524-019C-4CC1-8A7D-0E7C2C8338A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -825,7 +825,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,10 +941,14 @@
       <c r="B6" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6">
+        <v>4.4444444444444446E-2</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G6" s="21"/>
       <c r="H6" s="22"/>
       <c r="I6" s="4"/>

</xml_diff>

<commit_message>
solving for the T(n)
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B39524-019C-4CC1-8A7D-0E7C2C8338A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE687ECD-8915-42E5-A308-EFB22ADF4731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -458,7 +458,37 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -822,10 +852,10 @@
   <dimension ref="B1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,7 +908,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
@@ -901,7 +931,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
@@ -924,7 +954,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
@@ -947,7 +977,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="22"/>
@@ -964,10 +994,14 @@
       <c r="B7" s="5">
         <v>3.1</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>8.9583333333333334E-2</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G7" s="21"/>
       <c r="H7" s="22"/>
       <c r="I7" s="4"/>
@@ -983,10 +1017,14 @@
       <c r="B8" s="5">
         <v>3.2</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="22"/>
       <c r="I8" s="4"/>
@@ -1002,7 +1040,9 @@
       <c r="B9" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>4.583333333333333E-2</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
@@ -1017,7 +1057,9 @@
       <c r="B10" s="5">
         <v>4.2</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <v>4.583333333333333E-2</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
@@ -1625,14 +1667,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F52">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
-      <formula>0.89</formula>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
order of loops complete
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F680B1-B765-49D9-BF33-580C38B994D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A7D4BF-FBE7-46A3-BD73-59D9F9402D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -855,7 +855,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,10 +1078,14 @@
       <c r="B11" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>2.6388888888888889E-2</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
       <c r="I11" s="4"/>

</xml_diff>

<commit_message>
Order of nested for loops
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A7D4BF-FBE7-46A3-BD73-59D9F9402D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A56B5-8D28-48C5-B61C-60D64974323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -855,7 +855,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,10 +1097,14 @@
       <c r="B12" s="5">
         <v>5.2</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6">
+        <v>3.2638888888888891E-2</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
       <c r="I12" s="4"/>

</xml_diff>

<commit_message>
linear recursive relation complete
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A56B5-8D28-48C5-B61C-60D64974323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7749B17-30BB-4480-9C58-4D82428FEBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -855,7 +855,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,10 +1116,14 @@
       <c r="B13" s="5">
         <v>5.3</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6">
+        <v>3.6111111111111108E-2</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
       <c r="I13" s="4"/>

</xml_diff>

<commit_message>
adding solutions for RRs
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F72337-6DF9-4A0A-A706-94692CC37AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B50FE7-4572-41F7-B1EC-F22CDB743B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -458,68 +458,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -855,7 +794,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +939,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="22"/>
@@ -1023,7 +962,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="22"/>

</xml_diff>

<commit_message>
starting the topic of loops
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0E128B-B3AF-4CFB-9E7E-2A9C0CD7D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F226585D-5068-48F3-A0E6-3FE5666334EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -794,7 +794,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,7 +1004,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>

</xml_diff>

<commit_message>
solving for linear RRs
</commit_message>
<xml_diff>
--- a/DSA-Schedule.xlsx
+++ b/DSA-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F226585D-5068-48F3-A0E6-3FE5666334EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706EAFE-7E16-4751-95E9-FE1ED4D8BF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -794,7 +794,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1023,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
@@ -1042,7 +1042,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>

</xml_diff>